<commit_message>
refactor: merge test steps 1, 2, 3 & add delete cart item test
</commit_message>
<xml_diff>
--- a/doc/test_acceptation.xlsx
+++ b/doc/test_acceptation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="105">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Cliquer sur le produit "KANAP SINOPÈ".</t>
   </si>
   <si>
-    <t>En cliquant sur un produit, l'utilisateur sera redirigé sur la page du produit pour consulter celui-ci plus en détails.</t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
@@ -59,9 +56,6 @@
   </si>
   <si>
     <t>5.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">La page produit doit afficher l'image, le prix ainsi que la description du produit </t>
   </si>
   <si>
     <t>Relever l'affichage de l'image, le prix ainsi que la desciption pour le 
@@ -70,10 +64,6 @@
   <si>
     <t>Affichage de l'image, le prix ainsi que la desciption 
 pour  le produit "KANAP SINOPÈ".</t>
-  </si>
-  <si>
-    <t>La page produit doit avoir une liste déroulante permettant à l'utilisateur
-de choisir une option de personnalistion, ainsi qu’un input pour saisir la quantité.</t>
   </si>
   <si>
     <t>Sur la page produit, la possibilité d'ajouter un produit au panier.</t>
@@ -674,43 +664,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Saisir dans l'input "Qte" la quantité de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t xml:space="preserve">2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Montserrat"/>
-      </rPr>
-      <t>et relever le nombre total d'articles. Et le prix total.</t>
-    </r>
-  </si>
-  <si>
-    <t>8.1</t>
-  </si>
-  <si>
-    <t>8.2</t>
-  </si>
-  <si>
-    <t>8.3</t>
-  </si>
-  <si>
-    <t>8.4</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
     <t>Redirection vers la page qui affiche les détails du produit 
 "KANAP SINOPÈ".</t>
   </si>
@@ -719,10 +672,6 @@
   </si>
   <si>
     <t>Un message d'erreur affiché en dessous du champ email indiquant que l'adresse email n'est pas valide.</t>
-  </si>
-  <si>
-    <t>Validation des données saisies par les utilisateurs dans forumulaire de commande. Le prénom et le nom ne doivent  contenir que des lettres. 
-L'email doit êtres un email valide.</t>
   </si>
   <si>
     <t>Un message d'erreur affiché en dessous du prénom et nom indiquant que la valeur n'est pas valide et elle ne doit contenir que des lettres.</t>
@@ -1105,24 +1054,6 @@
     </r>
   </si>
   <si>
-    <t>9.1</t>
-  </si>
-  <si>
-    <t>9.2</t>
-  </si>
-  <si>
-    <t>9.3</t>
-  </si>
-  <si>
-    <t>9.4</t>
-  </si>
-  <si>
-    <t>9.5</t>
-  </si>
-  <si>
-    <t>9.6</t>
-  </si>
-  <si>
     <t xml:space="preserve">Affichage de l'ensemble des produits disponibles à la vente.
 </t>
   </si>
@@ -1131,9 +1062,6 @@
 "KANAP SINOPÈ".</t>
   </si>
   <si>
-    <t>Sur la page panier, l’utilisateur va pouvoir modifier la quantité d’un produit, à ce moment, le prix total et la quantité totale des produits du panier devront bien se mettre à jour.</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">
 La 1ère ligne affiche le le modèle "KANAP SINOPÈ" </t>
@@ -1213,9 +1141,6 @@
     </r>
   </si>
   <si>
-    <t>Aucune erreur dans le formurlaire de commande.</t>
-  </si>
-  <si>
     <t>Une redirection vers la page de confirmation.</t>
   </si>
   <si>
@@ -1271,13 +1196,105 @@
     <t>6.6</t>
   </si>
   <si>
-    <t>6.7</t>
-  </si>
-  <si>
-    <t>6.8</t>
-  </si>
-  <si>
-    <t>8.6</t>
+    <t>Aucune erreur dans le formulaire de commande.</t>
+  </si>
+  <si>
+    <t>Validation des données saisies par les utilisateurs dans formulaire de commande. Le prénom et le nom ne doivent  contenir que des lettres. 
+L'email doit êtres un email valide.</t>
+  </si>
+  <si>
+    <t>2.2</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>2.7</t>
+  </si>
+  <si>
+    <t>En cliquant sur un produit, l'utilisateur sera redirigé sur la page du produit pour consulter celui-ci plus en détails. La page produit doit afficher: 
+L'image, le prix, la description, ainsi qu'une liste déroulante permettant à l'utilisateur de choisir une option de personnalisation, ainsi qu'un input pour saisir la quantité</t>
+  </si>
+  <si>
+    <t>3.3</t>
+  </si>
+  <si>
+    <t>3.4</t>
+  </si>
+  <si>
+    <t>3.5</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>4.4</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
+    <t>4.6</t>
+  </si>
+  <si>
+    <t>4.7</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>7.6</t>
+  </si>
+  <si>
+    <t>Sur la page panier, l’utilisateur va pouvoir supprimer ou modifier la quantité d’un produit, à ce moment, le prix total et la quantité totale des produits du panier devront bien se mettre à jour. Les produits supprimés ne doivent plus être affichés.</t>
+  </si>
+  <si>
+    <t>Saisir dans l'input "Qte" la quantité de 2 et relever le nombre total d'articles. Et le prix total.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Aucun produit ne doit être affiché, le nombre total d'articles est à </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t xml:space="preserve"> et le prix total et à </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Montserrat"/>
+      </rPr>
+      <t>, une notification qui indique la supprision du produit.</t>
+    </r>
+  </si>
+  <si>
+    <t>Cliquer sur "Supprimer" et relever le nombre de produits affichés , le nombre total d'articles et le prix total.</t>
   </si>
 </sst>
 </file>
@@ -1394,7 +1411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1804,6 +1821,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1811,7 +1856,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1944,6 +1989,25 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="30" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2256,10 +2320,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E175"/>
+  <dimension ref="A1:E172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C56" sqref="C56"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="23.25" x14ac:dyDescent="0.35"/>
@@ -2291,7 +2355,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>5</v>
@@ -2305,14 +2369,14 @@
     </row>
     <row r="3" spans="1:5" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="25" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>4</v>
@@ -2320,16 +2384,16 @@
     </row>
     <row r="4" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
@@ -2337,32 +2401,32 @@
     </row>
     <row r="5" spans="1:5" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="B5" s="43"/>
       <c r="C5" s="43" t="s">
-        <v>92</v>
+        <v>74</v>
       </c>
       <c r="D5" s="43" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="12"/>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="52"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="54"/>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1" ht="226.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>2</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>10</v>
+        <v>90</v>
       </c>
       <c r="C7" s="20" t="s">
         <v>8</v>
@@ -2376,89 +2440,95 @@
     </row>
     <row r="8" spans="1:5" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B8" s="25"/>
       <c r="C8" s="20" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="11"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="12"/>
-    </row>
-    <row r="10" spans="1:5" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>3</v>
-      </c>
-      <c r="B10" s="25" t="s">
-        <v>15</v>
-      </c>
+    <row r="9" spans="1:5" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="25"/>
       <c r="C10" s="20" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>88</v>
       </c>
       <c r="B11" s="25"/>
       <c r="C11" s="20" t="s">
-        <v>80</v>
+        <v>14</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B12" s="25"/>
       <c r="C12" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="52"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="54"/>
+    </row>
+    <row r="14" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>3</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>4</v>
-      </c>
-      <c r="B14" s="25" t="s">
-        <v>18</v>
-      </c>
       <c r="C14" s="20" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>6</v>
@@ -2467,600 +2537,577 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B15" s="25"/>
       <c r="C15" s="20" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="B16" s="25"/>
       <c r="C16" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="19" t="s">
-        <v>36</v>
-      </c>
       <c r="E16" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="12"/>
-    </row>
-    <row r="18" spans="1:5" ht="100.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>5</v>
-      </c>
-      <c r="B18" s="25" t="s">
-        <v>19</v>
-      </c>
+    <row r="17" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="25"/>
       <c r="C18" s="20" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="D18" s="19" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="20" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="25"/>
+    <row r="20" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="52"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="53"/>
+      <c r="E20" s="54"/>
+    </row>
+    <row r="21" spans="1:5" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>4</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>27</v>
+      </c>
       <c r="C21" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="19"/>
+        <v>8</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="E21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="20" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="201" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>45</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="B23" s="27"/>
+      <c r="C23" s="40" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23" s="22"/>
       <c r="E23" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="35"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="12"/>
-    </row>
-    <row r="25" spans="1:5" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>6</v>
-      </c>
-      <c r="B25" s="25" t="s">
+    <row r="24" spans="1:5" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="28"/>
+      <c r="C24" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="C25" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="D24" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="30"/>
       <c r="E25" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>20</v>
+        <v>96</v>
       </c>
       <c r="B26" s="25"/>
       <c r="C26" s="20" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
       <c r="D26" s="19" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="201" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="40" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D27" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="D27" s="22"/>
       <c r="E27" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="200.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="B28" s="25"/>
+      <c r="C28" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B29" s="24"/>
-      <c r="C29" s="41" t="s">
-        <v>39</v>
-      </c>
-      <c r="D29" s="30"/>
+        <v>99</v>
+      </c>
+      <c r="B29" s="25"/>
+      <c r="C29" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="42" t="s">
+        <v>65</v>
+      </c>
       <c r="E29" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" s="25"/>
-      <c r="C30" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="102" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="52"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="53"/>
+      <c r="E30" s="54"/>
+    </row>
+    <row r="31" spans="1:5" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>5</v>
+      </c>
+      <c r="B31" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="25"/>
       <c r="C31" s="20" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D31" s="19" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="B32" s="25"/>
       <c r="C32" s="20" t="s">
-        <v>42</v>
+        <v>9</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="206.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>103</v>
+        <v>11</v>
       </c>
       <c r="B33" s="25"/>
       <c r="C33" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D33" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="D33" s="19"/>
+      <c r="E33" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" s="25"/>
+      <c r="C34" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="25"/>
+      <c r="C35" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="11"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="12"/>
-    </row>
-    <row r="35" spans="1:5" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>7</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>81</v>
-      </c>
-      <c r="C35" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="B36" s="25"/>
       <c r="C36" s="20" t="s">
-        <v>9</v>
+        <v>102</v>
       </c>
       <c r="D36" s="19" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B37" s="25"/>
-      <c r="C37" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D37" s="19"/>
-      <c r="E37" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B39" s="25"/>
+    <row r="37" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="51"/>
+      <c r="B37" s="49"/>
+      <c r="C37" s="48" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="50" t="s">
+        <v>103</v>
+      </c>
+      <c r="E37" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="52"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="53"/>
+      <c r="E38" s="54"/>
+    </row>
+    <row r="39" spans="1:5" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="5">
+        <v>6</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>85</v>
+      </c>
       <c r="C39" s="20" t="s">
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="B40" s="25"/>
       <c r="C40" s="20" t="s">
-        <v>54</v>
+        <v>9</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="11"/>
-      <c r="B41" s="26"/>
-      <c r="C41" s="35"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="12"/>
-    </row>
-    <row r="42" spans="1:5" ht="148.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="5">
-        <v>8</v>
-      </c>
-      <c r="B42" s="25" t="s">
-        <v>63</v>
-      </c>
+    <row r="41" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="25"/>
+      <c r="C41" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D41" s="19"/>
+      <c r="E41" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="25"/>
       <c r="C42" s="20" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="B43" s="25"/>
       <c r="C43" s="20" t="s">
-        <v>9</v>
+        <v>52</v>
       </c>
       <c r="D43" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44" s="25"/>
+      <c r="C44" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="171" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" s="25"/>
+      <c r="C45" s="38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="35"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="12"/>
+    </row>
+    <row r="47" spans="1:5" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="5">
+        <v>7</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B48" s="25"/>
+      <c r="C48" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B49" s="25"/>
+      <c r="C49" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="D49" s="19"/>
+      <c r="E49" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="25"/>
+      <c r="C50" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B51" s="25"/>
+      <c r="C51" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D44" s="19"/>
-      <c r="E44" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B46" s="25"/>
-      <c r="C46" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="25"/>
-      <c r="C47" s="38" t="s">
-        <v>67</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="171" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="B48" s="25"/>
-      <c r="C48" s="38" t="s">
-        <v>65</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="11"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="35"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="12"/>
-    </row>
-    <row r="50" spans="1:5" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="5">
-        <v>9</v>
-      </c>
-      <c r="B50" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B51" s="25"/>
-      <c r="C51" s="20" t="s">
-        <v>80</v>
-      </c>
       <c r="D51" s="19" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>74</v>
+        <v>47</v>
       </c>
       <c r="B52" s="25"/>
       <c r="C52" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D52" s="19"/>
+        <v>59</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="E52" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="87" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="B53" s="25"/>
       <c r="C53" s="20" t="s">
-        <v>37</v>
+        <v>62</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="185.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55" s="25"/>
-      <c r="C55" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B56" s="25"/>
-      <c r="C56" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
-      <c r="B57" s="29"/>
-      <c r="C57" s="36"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="15"/>
+    <row r="54" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="14"/>
+      <c r="B54" s="29"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="33"/>
+      <c r="E54" s="15"/>
+    </row>
+    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="16"/>
+      <c r="D55" s="17"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="16"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="16"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
@@ -3165,22 +3212,16 @@
       <c r="E74" s="1"/>
     </row>
     <row r="75" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="16"/>
-      <c r="D75" s="17"/>
-      <c r="E75" s="1"/>
+      <c r="A75"/>
+      <c r="E75"/>
     </row>
     <row r="76" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="16"/>
-      <c r="D76" s="17"/>
-      <c r="E76" s="1"/>
+      <c r="A76"/>
+      <c r="E76"/>
     </row>
     <row r="77" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="16"/>
-      <c r="D77" s="17"/>
-      <c r="E77" s="1"/>
+      <c r="A77"/>
+      <c r="E77"/>
     </row>
     <row r="78" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A78"/>
@@ -3446,58 +3487,55 @@
       <c r="A143"/>
       <c r="E143"/>
     </row>
-    <row r="144" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144"/>
-      <c r="E144"/>
-    </row>
-    <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145"/>
-      <c r="E145"/>
-    </row>
-    <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146"/>
-      <c r="E146"/>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147"/>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148"/>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A149"/>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150"/>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151"/>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152"/>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153"/>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154"/>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155"/>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156"/>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A157"/>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A158"/>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159"/>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A160"/>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.35">
@@ -3535,15 +3573,6 @@
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172"/>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A173"/>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A174"/>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A175"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>